<commit_message>
Fix header fixing countdown styling and align clock
</commit_message>
<xml_diff>
--- a/data/Stibor/GRSS/Nibor days 2026.xlsx
+++ b/data/Stibor/GRSS/Nibor days 2026.xlsx
@@ -10386,8 +10386,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x01010018D663DB1B96B8498A123F3887F55246" ma:contentTypeVersion="10" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="9fd2febd437389fd8a5d6c0b43c19e45">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d9c30b79-e6a1-4ed7-920c-5c2ba1b441f9" xmlns:ns3="f6c676c0-61b9-4e26-a136-e78363c7067a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b6e6c383851e65736407ef4fd265b8f8" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x01010018D663DB1B96B8498A123F3887F55246" ma:contentTypeVersion="10" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="19d493729cb5b1a8b93d4977cdad007b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d9c30b79-e6a1-4ed7-920c-5c2ba1b441f9" xmlns:ns3="f6c676c0-61b9-4e26-a136-e78363c7067a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a726f3ab3b3527a96921f3312a9b266d" ns2:_="" ns3:_="">
     <xsd:import namespace="d9c30b79-e6a1-4ed7-920c-5c2ba1b441f9"/>
     <xsd:import namespace="f6c676c0-61b9-4e26-a136-e78363c7067a"/>
     <xsd:element name="properties">
@@ -10595,7 +10595,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14AAE605-2D15-4E2D-A364-87602C2FBE44}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{446EAC70-54D7-4B42-9B7B-FB6BC17D82D1}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>